<commit_message>
Toujours + haut ...
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -1659,7 +1659,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43428</v>
+        <v>43436</v>
       </c>
     </row>
   </sheetData>
@@ -1789,10 +1789,10 @@
   <dimension ref="A2:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="11" ySplit="3" topLeftCell="L35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="3" topLeftCell="L43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J56" sqref="J56"/>
+      <selection pane="bottomRight" activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,12 +1843,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>634.93000000000006</v>
+        <v>643.23</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>1.0207877813504824</v>
+        <v>1.0341318327974276</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -3907,10 +3907,13 @@
         <f t="shared" si="61"/>
         <v>43436</v>
       </c>
-      <c r="J56" s="24"/>
+      <c r="J56" s="24">
+        <f xml:space="preserve"> 8.3</f>
+        <v>8.3000000000000007</v>
+      </c>
       <c r="K56" s="24">
         <f>SUM(J53:J56)</f>
-        <v>6.73</v>
+        <v>15.030000000000001</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Un peu plus haut
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018'!$B$3:$H$3</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1974,7 +1974,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43526</v>
+        <v>43541</v>
       </c>
     </row>
   </sheetData>
@@ -4498,7 +4498,7 @@
       <pane xSplit="11" ySplit="3" topLeftCell="L4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
+      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4548,12 +4548,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>62.17</v>
+        <v>78.819999999999993</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>9.9951768488745985E-2</v>
+        <v>0.12672025723472669</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -5121,7 +5121,10 @@
         <f t="shared" si="6"/>
         <v>43534</v>
       </c>
-      <c r="J18" s="24"/>
+      <c r="J18" s="24">
+        <f xml:space="preserve"> 8.93</f>
+        <v>8.93</v>
+      </c>
       <c r="K18" s="24"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -5157,7 +5160,10 @@
         <f t="shared" si="6"/>
         <v>43541</v>
       </c>
-      <c r="J19" s="24"/>
+      <c r="J19" s="24">
+        <f xml:space="preserve"> 7.72</f>
+        <v>7.72</v>
+      </c>
       <c r="K19" s="24"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -5232,7 +5238,7 @@
       <c r="J21" s="24"/>
       <c r="K21" s="24">
         <f>SUM(J18:J21)</f>
-        <v>0</v>
+        <v>16.649999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Corrigé avec merge manuel
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -1974,7 +1974,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43532</v>
+        <v>43545</v>
       </c>
     </row>
   </sheetData>
@@ -4498,7 +4498,7 @@
       <pane xSplit="11" ySplit="3" topLeftCell="L4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4548,12 +4548,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>71.099999999999994</v>
+        <v>82.949999999999989</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.11430868167202571</v>
+        <v>0.13336012861736332</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -5160,7 +5160,10 @@
         <f t="shared" si="6"/>
         <v>43541</v>
       </c>
-      <c r="J19" s="24"/>
+      <c r="J19" s="24">
+        <f xml:space="preserve"> 7.72</f>
+        <v>7.72</v>
+      </c>
       <c r="K19" s="24"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -5196,7 +5199,10 @@
         <f t="shared" si="8"/>
         <v>43548</v>
       </c>
-      <c r="J20" s="24"/>
+      <c r="J20" s="24">
+        <f xml:space="preserve"> 4.13</f>
+        <v>4.13</v>
+      </c>
       <c r="K20" s="24"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -5235,7 +5241,7 @@
       <c r="J21" s="24"/>
       <c r="K21" s="24">
         <f>SUM(J18:J21)</f>
-        <v>8.93</v>
+        <v>20.779999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Et de trois dans la semaine ...
... Genoux toujours en délicatesse, surtout le gauche aujourd'hui. Ne surtout pas forcer l'allure. Musculature toujours insuffisante aux deux genoux
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -4548,12 +4548,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>89.169999999999987</v>
+        <v>96.259999999999991</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.14336012861736333</v>
+        <v>0.15475884244372989</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -5200,8 +5200,8 @@
         <v>43548</v>
       </c>
       <c r="J20" s="24">
-        <f xml:space="preserve"> 4.13 + 6.22</f>
-        <v>10.35</v>
+        <f xml:space="preserve"> 4.13 + 6.22 + 7.09</f>
+        <v>17.439999999999998</v>
       </c>
       <c r="K20" s="24"/>
     </row>
@@ -5241,7 +5241,7 @@
       <c r="J21" s="24"/>
       <c r="K21" s="24">
         <f>SUM(J18:J21)</f>
-        <v>27</v>
+        <v>34.089999999999996</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
7% de retard ...
Très dur cet après-midi ...
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -1974,7 +1974,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43554</v>
+        <v>43555</v>
       </c>
     </row>
   </sheetData>
@@ -4548,12 +4548,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>108.69999999999999</v>
+        <v>115.32999999999998</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.17475884244372988</v>
+        <v>0.18541800643086814</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -5239,12 +5239,12 @@
         <v>43555</v>
       </c>
       <c r="J21" s="24">
-        <f xml:space="preserve"> 6.26 + 6.18</f>
-        <v>12.44</v>
+        <f xml:space="preserve"> 6.26 + 6.18 + 6.63</f>
+        <v>19.07</v>
       </c>
       <c r="K21" s="24">
         <f>SUM(J18:J21)</f>
-        <v>46.529999999999994</v>
+        <v>53.16</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Et de deux ...
... en deux jours
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -4495,7 +4495,7 @@
   <dimension ref="A2:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="11" ySplit="3" topLeftCell="L11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="3" topLeftCell="L15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
@@ -4548,12 +4548,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>134.14999999999998</v>
+        <v>142.29999999999998</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.21567524115755624</v>
+        <v>0.2287781350482315</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -5320,8 +5320,8 @@
         <v>43569</v>
       </c>
       <c r="J23" s="24">
-        <f xml:space="preserve"> 7.55</f>
-        <v>7.55</v>
+        <f xml:space="preserve"> 7.55 + 8.15</f>
+        <v>15.7</v>
       </c>
       <c r="K23" s="24"/>
     </row>
@@ -5433,7 +5433,7 @@
       <c r="J26" s="24"/>
       <c r="K26" s="24">
         <f>SUM(J22:J26)</f>
-        <v>18.82</v>
+        <v>26.97</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
De l'or de avril
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -1974,7 +1974,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43576</v>
+        <v>43582</v>
       </c>
     </row>
   </sheetData>
@@ -4498,7 +4498,7 @@
       <pane xSplit="11" ySplit="3" topLeftCell="L15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J24" sqref="J24"/>
+      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4548,12 +4548,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>160.1</v>
+        <v>168.74</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.25739549839228293</v>
+        <v>0.27128617363344054</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -5397,7 +5397,10 @@
         <f t="shared" si="8"/>
         <v>43583</v>
       </c>
-      <c r="J25" s="24"/>
+      <c r="J25" s="24">
+        <f xml:space="preserve"> 8.64</f>
+        <v>8.64</v>
+      </c>
       <c r="K25" s="24"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -5436,7 +5439,7 @@
       <c r="J26" s="24"/>
       <c r="K26" s="24">
         <f>SUM(J22:J26)</f>
-        <v>44.769999999999996</v>
+        <v>53.41</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Si près du tiers
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -1974,7 +1974,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43590</v>
+        <v>43593</v>
       </c>
     </row>
   </sheetData>
@@ -4498,7 +4498,7 @@
       <pane xSplit="11" ySplit="3" topLeftCell="L15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
+      <selection pane="bottomRight" activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4548,12 +4548,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>197.75</v>
+        <v>205.07</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.31792604501607719</v>
+        <v>0.32969453376205787</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -5478,7 +5478,10 @@
         <f t="shared" si="8"/>
         <v>43597</v>
       </c>
-      <c r="J27" s="24"/>
+      <c r="J27" s="24">
+        <f xml:space="preserve"> 7.32</f>
+        <v>7.32</v>
+      </c>
       <c r="K27" s="24"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -5589,7 +5592,7 @@
       <c r="J30" s="24"/>
       <c r="K30" s="24">
         <f>SUM(J27:J30)</f>
-        <v>0</v>
+        <v>7.32</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Le premier tiers ...
.. plus que deux semaines de retard ...
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -1974,7 +1974,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43593</v>
+        <v>43596</v>
       </c>
     </row>
   </sheetData>
@@ -4548,12 +4548,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>205.07</v>
+        <v>212.4</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.32969453376205787</v>
+        <v>0.34147909967845658</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -5479,8 +5479,8 @@
         <v>43597</v>
       </c>
       <c r="J27" s="24">
-        <f xml:space="preserve"> 7.32</f>
-        <v>7.32</v>
+        <f xml:space="preserve"> 7.32 + 7.33</f>
+        <v>14.65</v>
       </c>
       <c r="K27" s="24"/>
     </row>
@@ -5592,7 +5592,7 @@
       <c r="J30" s="24"/>
       <c r="K30" s="24">
         <f>SUM(J27:J30)</f>
-        <v>7.32</v>
+        <v>14.65</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Première course de juin
... pas facile !
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018'!$B$3:$H$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -1974,7 +1974,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43615</v>
+        <v>43618</v>
       </c>
     </row>
   </sheetData>
@@ -4548,12 +4548,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>243.83</v>
+        <v>252.21</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.39200964630225082</v>
+        <v>0.40548231511254018</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -5596,12 +5596,12 @@
         <v>43618</v>
       </c>
       <c r="J30" s="24">
-        <f xml:space="preserve"> 7.71</f>
-        <v>7.71</v>
+        <f xml:space="preserve"> 7.71 + 8.38</f>
+        <v>16.09</v>
       </c>
       <c r="K30" s="24">
         <f>SUM(J27:J30)</f>
-        <v>46.08</v>
+        <v>54.459999999999994</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
60 km de la mi-saison
1 mois ?
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -1974,7 +1974,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43624</v>
+        <v>43632</v>
       </c>
     </row>
   </sheetData>
@@ -4498,7 +4498,7 @@
       <pane xSplit="11" ySplit="3" topLeftCell="L18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J31" sqref="J31"/>
+      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4548,12 +4548,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>266.89</v>
+        <v>274.43</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.42908360128617362</v>
+        <v>0.4412057877813505</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -5676,7 +5676,10 @@
         <f t="shared" si="10"/>
         <v>43632</v>
       </c>
-      <c r="J32" s="24"/>
+      <c r="J32" s="24">
+        <f xml:space="preserve"> 7.54</f>
+        <v>7.54</v>
+      </c>
       <c r="K32" s="24"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -5751,7 +5754,7 @@
       <c r="J34" s="24"/>
       <c r="K34" s="24">
         <f>SUM(J31:J34)</f>
-        <v>14.68</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Encore 3 courses ...
... pour atteindre la mi-course ...
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -1974,7 +1974,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43639</v>
+        <v>43646</v>
       </c>
     </row>
   </sheetData>
@@ -4498,7 +4498,7 @@
       <pane xSplit="11" ySplit="3" topLeftCell="L18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J33" sqref="J33"/>
+      <selection pane="bottomRight" activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4548,12 +4548,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>287.3</v>
+        <v>295.35000000000002</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.46189710610932477</v>
+        <v>0.47483922829581998</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -5754,10 +5754,13 @@
         <f t="shared" si="10"/>
         <v>43646</v>
       </c>
-      <c r="J34" s="24"/>
+      <c r="J34" s="24">
+        <f xml:space="preserve"> 8.05</f>
+        <v>8.0500000000000007</v>
+      </c>
       <c r="K34" s="24">
         <f>SUM(J31:J34)</f>
-        <v>35.089999999999996</v>
+        <v>43.14</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
On approche de ma mi-course
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -1974,7 +1974,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43646</v>
+        <v>43652</v>
       </c>
     </row>
   </sheetData>
@@ -4498,7 +4498,7 @@
       <pane xSplit="11" ySplit="3" topLeftCell="L18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J34" sqref="J34"/>
+      <selection pane="bottomRight" activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4548,12 +4548,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>295.35000000000002</v>
+        <v>303.43</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.47483922829581998</v>
+        <v>0.48782958199356913</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -5796,7 +5796,10 @@
         <f t="shared" si="10"/>
         <v>43653</v>
       </c>
-      <c r="J35" s="24"/>
+      <c r="J35" s="24">
+        <f xml:space="preserve"> 8.08</f>
+        <v>8.08</v>
+      </c>
       <c r="K35" s="24"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -5943,7 +5946,7 @@
       <c r="J39" s="24"/>
       <c r="K39" s="24">
         <f>SUM(J35:J39)</f>
-        <v>0</v>
+        <v>8.08</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Première de la semaine
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018'!$B$3:$H$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -1974,7 +1974,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43660</v>
+        <v>43661</v>
       </c>
     </row>
   </sheetData>
@@ -4498,7 +4498,7 @@
       <pane xSplit="11" ySplit="3" topLeftCell="L19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J36" sqref="J36"/>
+      <selection pane="bottomRight" activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4548,12 +4548,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>319.82</v>
+        <v>326.08</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.51418006430868168</v>
+        <v>0.52424437299035365</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -5874,7 +5874,10 @@
         <f t="shared" si="10"/>
         <v>43667</v>
       </c>
-      <c r="J37" s="24"/>
+      <c r="J37" s="24">
+        <f xml:space="preserve"> 6.26</f>
+        <v>6.26</v>
+      </c>
       <c r="K37" s="24"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -5949,7 +5952,7 @@
       <c r="J39" s="24"/>
       <c r="K39" s="24">
         <f>SUM(J35:J39)</f>
-        <v>24.47</v>
+        <v>30.729999999999997</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Le mois n'est peut-être pas fini ...
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -1974,7 +1974,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43666</v>
+        <v>43674</v>
       </c>
     </row>
   </sheetData>
@@ -4498,7 +4498,7 @@
       <pane xSplit="11" ySplit="3" topLeftCell="L19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J37" sqref="J37"/>
+      <selection pane="bottomRight" activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4548,12 +4548,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>341.19</v>
+        <v>372.05999999999995</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.5485369774919614</v>
+        <v>0.59816720257234723</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -5875,8 +5875,8 @@
         <v>43667</v>
       </c>
       <c r="J37" s="24">
-        <f xml:space="preserve"> 6.26 + 6.47 + 8.64</f>
-        <v>21.37</v>
+        <f xml:space="preserve"> 6.26 + 6.47 + 8.64 + 7.78</f>
+        <v>29.150000000000002</v>
       </c>
       <c r="K37" s="24"/>
     </row>
@@ -5913,7 +5913,10 @@
         <f t="shared" si="12"/>
         <v>43674</v>
       </c>
-      <c r="J38" s="24"/>
+      <c r="J38" s="24">
+        <f xml:space="preserve"> 5.66 + 8.24 + 9.19</f>
+        <v>23.09</v>
+      </c>
       <c r="K38" s="24"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -5952,7 +5955,7 @@
       <c r="J39" s="24"/>
       <c r="K39" s="24">
         <f>SUM(J35:J39)</f>
-        <v>45.84</v>
+        <v>76.710000000000008</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
encore 300 km ...
... une trentaine de courses, 8 semaines ? 2 mois ?
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -1974,7 +1974,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43697</v>
+        <v>43701</v>
       </c>
     </row>
   </sheetData>
@@ -4548,12 +4548,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>429.04999999999995</v>
+        <v>439.24999999999994</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.68979099678456579</v>
+        <v>0.70618971061093239</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -6072,7 +6072,10 @@
         <f t="shared" si="14"/>
         <v>43702</v>
       </c>
-      <c r="J42" s="24"/>
+      <c r="J42" s="24">
+        <f xml:space="preserve"> 10.2</f>
+        <v>10.199999999999999</v>
+      </c>
       <c r="K42" s="24"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -6111,7 +6114,7 @@
       <c r="J43" s="24"/>
       <c r="K43" s="24">
         <f>SUM(J40:J43)</f>
-        <v>49.66</v>
+        <v>59.86</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Vite mais dur dur
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -1974,7 +1974,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43724</v>
+        <v>43727</v>
       </c>
     </row>
   </sheetData>
@@ -4548,12 +4548,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>457.06999999999994</v>
+        <v>464.50999999999993</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.73483922829581982</v>
+        <v>0.7468006430868166</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -6225,7 +6225,10 @@
         <f t="shared" si="14"/>
         <v>43730</v>
       </c>
-      <c r="J46" s="24"/>
+      <c r="J46" s="24">
+        <f xml:space="preserve"> 7.44</f>
+        <v>7.44</v>
+      </c>
       <c r="K46" s="24"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -6264,7 +6267,7 @@
       <c r="J47" s="24"/>
       <c r="K47" s="24">
         <f>SUM(J44:J47)</f>
-        <v>9.51</v>
+        <v>16.95</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
100 miles trop court
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018'!$B$3:$H$3</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1974,7 +1974,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43814</v>
+        <v>43824</v>
       </c>
     </row>
   </sheetData>
@@ -4495,10 +4495,10 @@
   <dimension ref="A2:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="11" ySplit="3" topLeftCell="L39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="3" topLeftCell="L45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J58" sqref="J58"/>
+      <selection pane="bottomRight" activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4548,12 +4548,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>514.42999999999995</v>
+        <v>522.07999999999993</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.8270578778135047</v>
+        <v>0.83935691318327965</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -6756,7 +6756,9 @@
         <f t="shared" si="20"/>
         <v>43828</v>
       </c>
-      <c r="J60" s="24"/>
+      <c r="J60" s="24">
+        <v>7.65</v>
+      </c>
       <c r="K60" s="24"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -6795,7 +6797,7 @@
       <c r="J61" s="24"/>
       <c r="K61" s="24">
         <f>SUM(J57:J61)</f>
-        <v>20.77</v>
+        <v>28.42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Barre des 50 premiers km franchie ...
... au pas de course ;-)
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -2295,7 +2295,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43846</v>
+        <v>43849</v>
       </c>
     </row>
   </sheetData>
@@ -7248,12 +7248,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>26.240000000000002</v>
+        <v>32.660000000000004</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>4.218649517684888E-2</v>
+        <v>5.2508038585209006E-2</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -7552,8 +7552,8 @@
         <v>43849</v>
       </c>
       <c r="J11" s="24">
-        <f xml:space="preserve"> 6.23</f>
-        <v>6.23</v>
+        <f xml:space="preserve"> 6.23 + 6.42</f>
+        <v>12.65</v>
       </c>
       <c r="K11" s="24"/>
     </row>
@@ -7629,7 +7629,7 @@
       <c r="J13" s="24"/>
       <c r="K13" s="24">
         <f>SUM(J9:J13)</f>
-        <v>26.240000000000002</v>
+        <v>32.660000000000004</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Début du second mois
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -2295,7 +2295,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43849</v>
+        <v>43862</v>
       </c>
     </row>
   </sheetData>
@@ -7198,7 +7198,7 @@
   <dimension ref="A2:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7248,12 +7248,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>32.660000000000004</v>
+        <v>46.74</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>5.2508038585209006E-2</v>
+        <v>7.514469453376206E-2</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -7590,7 +7590,10 @@
         <f xml:space="preserve"> Tableau145[[#This Row],[Samedi]] + 1</f>
         <v>43856</v>
       </c>
-      <c r="J12" s="24"/>
+      <c r="J12" s="24">
+        <f>6.29</f>
+        <v>6.29</v>
+      </c>
       <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -7626,10 +7629,12 @@
         <f xml:space="preserve"> Tableau145[[#This Row],[Samedi]] + 1</f>
         <v>43863</v>
       </c>
-      <c r="J13" s="24"/>
+      <c r="J13" s="24">
+        <v>7.79</v>
+      </c>
       <c r="K13" s="24">
         <f>SUM(J9:J13)</f>
-        <v>32.660000000000004</v>
+        <v>46.74</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
15% et au delà
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -16,7 +16,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018'!$B$3:$H$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -2295,7 +2295,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43890</v>
+        <v>43894</v>
       </c>
     </row>
   </sheetData>
@@ -7198,7 +7198,7 @@
   <dimension ref="A2:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7248,12 +7248,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>90.37</v>
+        <v>94.62</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.14528938906752412</v>
+        <v>0.15212218649517686</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -7829,7 +7829,10 @@
         <f xml:space="preserve"> Tableau145[[#This Row],[Samedi]] + 1</f>
         <v>43898</v>
       </c>
-      <c r="J18" s="24"/>
+      <c r="J18" s="24">
+        <f xml:space="preserve"> 4.25</f>
+        <v>4.25</v>
+      </c>
       <c r="K18" s="24"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -7940,7 +7943,7 @@
       <c r="J21" s="24"/>
       <c r="K21" s="24">
         <f>SUM(J18:J21)</f>
-        <v>0</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
1/5, en route !
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -2295,7 +2295,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43904</v>
+        <v>43905</v>
       </c>
     </row>
   </sheetData>
@@ -7248,12 +7248,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>121.54</v>
+        <v>131.66</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.19540192926045016</v>
+        <v>0.21167202572347266</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -7869,8 +7869,8 @@
         <v>43905</v>
       </c>
       <c r="J19" s="24">
-        <f xml:space="preserve"> 10.06</f>
-        <v>10.06</v>
+        <f xml:space="preserve"> 10.06 + 10.12</f>
+        <v>20.18</v>
       </c>
       <c r="K19" s="24"/>
     </row>
@@ -7946,7 +7946,7 @@
       <c r="J21" s="24"/>
       <c r="K21" s="24">
         <f>SUM(J18:J21)</f>
-        <v>31.17</v>
+        <v>41.29</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
un pas plus loin ...
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -2295,7 +2295,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43908</v>
+        <v>43909</v>
       </c>
     </row>
   </sheetData>
@@ -7248,12 +7248,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>142.24</v>
+        <v>152.28</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.22868167202572348</v>
+        <v>0.24482315112540193</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -7908,7 +7908,8 @@
         <v>43912</v>
       </c>
       <c r="J20" s="24">
-        <v>10.58</v>
+        <f xml:space="preserve"> 10.58 + 10.04</f>
+        <v>20.619999999999997</v>
       </c>
       <c r="K20" s="24"/>
     </row>
@@ -7948,7 +7949,7 @@
       <c r="J21" s="24"/>
       <c r="K21" s="24">
         <f>SUM(J18:J21)</f>
-        <v>51.87</v>
+        <v>61.91</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
A quelques pas de ....
... 300 km
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -16,7 +16,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018'!$B$3:$H$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -2295,7 +2295,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43912</v>
+        <v>43917</v>
       </c>
     </row>
   </sheetData>
@@ -7198,7 +7198,7 @@
   <dimension ref="A2:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7248,12 +7248,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>163.59</v>
+        <v>185.69</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.26300643086816722</v>
+        <v>0.2985369774919614</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -7946,10 +7946,13 @@
         <f xml:space="preserve"> Tableau145[[#This Row],[Samedi]] + 1</f>
         <v>43919</v>
       </c>
-      <c r="J21" s="24"/>
+      <c r="J21" s="24">
+        <f xml:space="preserve"> 10.62 + 11.48</f>
+        <v>22.1</v>
+      </c>
       <c r="K21" s="24">
         <f>SUM(J18:J21)</f>
-        <v>73.22</v>
+        <v>95.32</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pas tout à fait au tiers
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -2295,7 +2295,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43917</v>
+        <v>43924</v>
       </c>
     </row>
   </sheetData>
@@ -7198,7 +7198,7 @@
   <dimension ref="A2:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7248,12 +7248,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>185.69</v>
+        <v>202.77</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.2985369774919614</v>
+        <v>0.32599678456591641</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -7988,7 +7988,10 @@
         <f xml:space="preserve"> Tableau145[[#This Row],[Samedi]] + 1</f>
         <v>43926</v>
       </c>
-      <c r="J22" s="24"/>
+      <c r="J22" s="24">
+        <f xml:space="preserve"> 7.03 + 10.05</f>
+        <v>17.080000000000002</v>
+      </c>
       <c r="K22" s="24"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -8135,7 +8138,7 @@
       <c r="J26" s="24"/>
       <c r="K26" s="24">
         <f>SUM(J22:J26)</f>
-        <v>0</v>
+        <v>17.080000000000002</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
A deux courses de la mi-parcours
... en 5 mois ...
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -16,7 +16,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018'!$B$3:$H$3</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -2295,7 +2295,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43968</v>
+        <v>43973</v>
       </c>
     </row>
   </sheetData>
@@ -7201,7 +7201,7 @@
       <pane xSplit="8" ySplit="3" topLeftCell="I13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J28" sqref="J28"/>
+      <selection pane="bottomRight" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7251,12 +7251,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>288.83999999999997</v>
+        <v>302.85999999999996</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.46437299035369772</v>
+        <v>0.4869131832797427</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -8264,7 +8264,10 @@
         <f xml:space="preserve"> Tableau145[[#This Row],[Samedi]] + 1</f>
         <v>43975</v>
       </c>
-      <c r="J29" s="24"/>
+      <c r="J29" s="24">
+        <f xml:space="preserve"> 6.9 +7.12</f>
+        <v>14.02</v>
+      </c>
       <c r="K29" s="24"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -8303,7 +8306,7 @@
       <c r="J30" s="24"/>
       <c r="K30" s="24">
         <f>SUM(J27:J30)</f>
-        <v>35.56</v>
+        <v>49.58</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Descente en cours ...
... tout juste
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -16,7 +16,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018'!$B$3:$H$3</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -2295,7 +2295,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43975</v>
+        <v>43977</v>
       </c>
     </row>
   </sheetData>
@@ -7201,7 +7201,7 @@
       <pane xSplit="8" ySplit="3" topLeftCell="I13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J29" sqref="J29"/>
+      <selection pane="bottomRight" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7251,12 +7251,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>311.53999999999996</v>
+        <v>318.47999999999996</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.50086816720257232</v>
+        <v>0.51202572347266873</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -8303,10 +8303,13 @@
         <f xml:space="preserve"> Tableau145[[#This Row],[Samedi]] + 1</f>
         <v>43982</v>
       </c>
-      <c r="J30" s="24"/>
+      <c r="J30" s="24">
+        <f xml:space="preserve"> 6.94</f>
+        <v>6.94</v>
+      </c>
       <c r="K30" s="24">
         <f>SUM(J27:J30)</f>
-        <v>58.260000000000005</v>
+        <v>65.2</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Niveau NOIR ! désormais dans Nike+
... Comme c'est sombre, tout ce NOIR !
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -2304,7 +2304,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>44029</v>
+        <v>44033</v>
       </c>
     </row>
   </sheetData>
@@ -7263,20 +7263,20 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>419.10999999999996</v>
+        <v>427.53999999999996</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.67381028938906751</v>
+        <v>0.68736334405144683</v>
       </c>
       <c r="M3" s="29">
         <f xml:space="preserve"> $J$3 - $L$2</f>
-        <v>-202.89000000000004</v>
+        <v>-194.46000000000004</v>
       </c>
       <c r="N3" s="30">
         <f xml:space="preserve"> $M$3 / $L$2 * 1000</f>
-        <v>-326.18971061093254</v>
+        <v>-312.63665594855308</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -8601,7 +8601,8 @@
         <v>44031</v>
       </c>
       <c r="J37" s="24">
-        <v>9.01</v>
+        <f xml:space="preserve"> 9.01 + 8.43</f>
+        <v>17.439999999999998</v>
       </c>
       <c r="K37" s="24"/>
     </row>
@@ -8677,7 +8678,7 @@
       <c r="J39" s="24"/>
       <c r="K39" s="24">
         <f>SUM(J35:J39)</f>
-        <v>25.21</v>
+        <v>33.64</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
280 km à parcourir ...
... ça fait quelques marathons
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -2304,7 +2304,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>44037</v>
+        <v>44038</v>
       </c>
     </row>
   </sheetData>
@@ -7263,20 +7263,20 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>442.46999999999997</v>
+        <v>447.90999999999997</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.71136655948553051</v>
+        <v>0.72011254019292603</v>
       </c>
       <c r="M3" s="29">
         <f xml:space="preserve"> $J$3 - $L$2</f>
-        <v>-179.53000000000003</v>
+        <v>-174.09000000000003</v>
       </c>
       <c r="N3" s="30">
         <f xml:space="preserve"> $M$3 / $L$2 * 1000</f>
-        <v>-288.6334405144695</v>
+        <v>-279.88745980707404</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -8640,8 +8640,8 @@
         <v>44038</v>
       </c>
       <c r="J38" s="24">
-        <f xml:space="preserve"> 14.93</f>
-        <v>14.93</v>
+        <f xml:space="preserve"> 14.93 + 5.44</f>
+        <v>20.37</v>
       </c>
       <c r="K38" s="24"/>
     </row>
@@ -8681,7 +8681,7 @@
       <c r="J39" s="24"/>
       <c r="K39" s="24">
         <f>SUM(J35:J39)</f>
-        <v>48.57</v>
+        <v>54.010000000000005</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
5 months to go
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -2304,7 +2304,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>44038</v>
+        <v>44044</v>
       </c>
     </row>
   </sheetData>
@@ -7210,7 +7210,7 @@
       <pane xSplit="8" ySplit="3" topLeftCell="J25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J38" sqref="J38"/>
+      <selection pane="bottomRight" activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7263,20 +7263,20 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>447.90999999999997</v>
+        <v>456.59999999999997</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.72011254019292603</v>
+        <v>0.73408360128617356</v>
       </c>
       <c r="M3" s="29">
         <f xml:space="preserve"> $J$3 - $L$2</f>
-        <v>-174.09000000000003</v>
+        <v>-165.40000000000003</v>
       </c>
       <c r="N3" s="30">
         <f xml:space="preserve"> $M$3 / $L$2 * 1000</f>
-        <v>-279.88745980707404</v>
+        <v>-265.91639871382642</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -8678,10 +8678,13 @@
         <f xml:space="preserve"> Tableau145[[#This Row],[Samedi]] + 1</f>
         <v>44045</v>
       </c>
-      <c r="J39" s="24"/>
+      <c r="J39" s="24">
+        <f xml:space="preserve"> 8.69</f>
+        <v>8.69</v>
+      </c>
       <c r="K39" s="24">
         <f>SUM(J35:J39)</f>
-        <v>54.010000000000005</v>
+        <v>62.7</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Nous frisons les 4/5
Encore un effort ...
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -2304,7 +2304,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>44071</v>
+        <v>44073</v>
       </c>
     </row>
   </sheetData>
@@ -7207,7 +7207,7 @@
   <dimension ref="A2:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="3" topLeftCell="J25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="3" topLeftCell="J32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="J43" sqref="J43"/>
@@ -7263,20 +7263,20 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>484.71</v>
+        <v>494.78</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.77927652733118968</v>
+        <v>0.79546623794212212</v>
       </c>
       <c r="M3" s="29">
         <f xml:space="preserve"> $J$3 - $L$2</f>
-        <v>-137.29000000000002</v>
+        <v>-127.22000000000003</v>
       </c>
       <c r="N3" s="30">
         <f xml:space="preserve"> $M$3 / $L$2 * 1000</f>
-        <v>-220.7234726688103</v>
+        <v>-204.53376205787785</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -8832,12 +8832,12 @@
         <v>44073</v>
       </c>
       <c r="J43" s="24">
-        <f xml:space="preserve"> 6.89 + 6.55</f>
-        <v>13.44</v>
+        <f xml:space="preserve"> 6.89 + 6.55 + 10.07</f>
+        <v>23.509999999999998</v>
       </c>
       <c r="K43" s="24">
         <f>SUM(J40:J43)</f>
-        <v>28.11</v>
+        <v>38.18</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
A moins de 200 km du but ...
... une vingtaine de courses ...
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -2304,7 +2304,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>44073</v>
+        <v>44083</v>
       </c>
     </row>
   </sheetData>
@@ -7210,7 +7210,7 @@
       <pane xSplit="8" ySplit="3" topLeftCell="J32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J43" sqref="J43"/>
+      <selection pane="bottomRight" activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7263,20 +7263,20 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>494.78</v>
+        <v>501.71</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.79546623794212212</v>
+        <v>0.80660771704180056</v>
       </c>
       <c r="M3" s="29">
         <f xml:space="preserve"> $J$3 - $L$2</f>
-        <v>-127.22000000000003</v>
+        <v>-120.29000000000002</v>
       </c>
       <c r="N3" s="30">
         <f xml:space="preserve"> $M$3 / $L$2 * 1000</f>
-        <v>-204.53376205787785</v>
+        <v>-193.39228295819939</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -8909,7 +8909,10 @@
         <f xml:space="preserve"> Tableau145[[#This Row],[Samedi]] + 1</f>
         <v>44087</v>
       </c>
-      <c r="J45" s="24"/>
+      <c r="J45" s="24">
+        <f xml:space="preserve"> 6.93</f>
+        <v>6.93</v>
+      </c>
       <c r="K45" s="24"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -8984,7 +8987,7 @@
       <c r="J47" s="24"/>
       <c r="K47" s="24">
         <f>SUM(J44:J47)</f>
-        <v>0</v>
+        <v>6.93</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Encore 140 km ...
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -2304,7 +2304,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>44092</v>
+        <v>44094</v>
       </c>
     </row>
   </sheetData>
@@ -7263,20 +7263,20 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>526.12</v>
+        <v>534.59</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.84585209003215434</v>
+        <v>0.85946945337620584</v>
       </c>
       <c r="M3" s="29">
         <f xml:space="preserve"> $J$3 - $L$2</f>
-        <v>-95.88</v>
+        <v>-87.409999999999968</v>
       </c>
       <c r="N3" s="30">
         <f xml:space="preserve"> $M$3 / $L$2 * 1000</f>
-        <v>-154.14790996784566</v>
+        <v>-140.53054662379415</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -8949,8 +8949,8 @@
         <v>44094</v>
       </c>
       <c r="J46" s="24">
-        <f xml:space="preserve"> 7.24</f>
-        <v>7.24</v>
+        <f xml:space="preserve"> 7.24 + 8.47</f>
+        <v>15.71</v>
       </c>
       <c r="K46" s="24"/>
     </row>
@@ -8990,7 +8990,7 @@
       <c r="J47" s="24"/>
       <c r="K47" s="24">
         <f>SUM(J44:J47)</f>
-        <v>31.340000000000003</v>
+        <v>39.81</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
80 mi to go ...
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -2304,7 +2304,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>44094</v>
+        <v>44096</v>
       </c>
     </row>
   </sheetData>
@@ -7210,7 +7210,7 @@
       <pane xSplit="8" ySplit="3" topLeftCell="J32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J46" sqref="J46"/>
+      <selection pane="bottomRight" activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7263,20 +7263,20 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>534.59</v>
+        <v>541.98</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.85946945337620584</v>
+        <v>0.87135048231511258</v>
       </c>
       <c r="M3" s="29">
         <f xml:space="preserve"> $J$3 - $L$2</f>
-        <v>-87.409999999999968</v>
+        <v>-80.019999999999982</v>
       </c>
       <c r="N3" s="30">
         <f xml:space="preserve"> $M$3 / $L$2 * 1000</f>
-        <v>-140.53054662379415</v>
+        <v>-128.64951768488746</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -8987,10 +8987,13 @@
         <f xml:space="preserve"> Tableau145[[#This Row],[Samedi]] + 1</f>
         <v>44101</v>
       </c>
-      <c r="J47" s="24"/>
+      <c r="J47" s="24">
+        <f xml:space="preserve"> 7.39</f>
+        <v>7.39</v>
+      </c>
       <c r="K47" s="24">
         <f>SUM(J44:J47)</f>
-        <v>39.81</v>
+        <v>47.2</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Moins de 100 km du but
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -2304,7 +2304,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>44097</v>
+        <v>44108</v>
       </c>
     </row>
   </sheetData>
@@ -7210,7 +7210,7 @@
       <pane xSplit="8" ySplit="3" topLeftCell="J32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J47" sqref="J47"/>
+      <selection pane="bottomRight" activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7263,20 +7263,20 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>549.6</v>
+        <v>564.08000000000004</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.88360128617363343</v>
+        <v>0.90688102893890676</v>
       </c>
       <c r="M3" s="29">
         <f xml:space="preserve"> $J$3 - $L$2</f>
-        <v>-72.399999999999977</v>
+        <v>-57.919999999999959</v>
       </c>
       <c r="N3" s="30">
         <f xml:space="preserve"> $M$3 / $L$2 * 1000</f>
-        <v>-116.39871382636652</v>
+        <v>-93.118971061093177</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -9029,7 +9029,10 @@
         <f xml:space="preserve"> Tableau145[[#This Row],[Samedi]] + 1</f>
         <v>44108</v>
       </c>
-      <c r="J48" s="24"/>
+      <c r="J48" s="24">
+        <f xml:space="preserve"> 6.4 + 8.08</f>
+        <v>14.48</v>
+      </c>
       <c r="K48" s="24"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -9176,7 +9179,7 @@
       <c r="J52" s="24"/>
       <c r="K52" s="24">
         <f>SUM(J48:J52)</f>
-        <v>0</v>
+        <v>14.48</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
reste 82 km à parcourir
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -2304,7 +2304,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>44108</v>
+        <v>44111</v>
       </c>
     </row>
   </sheetData>
@@ -7210,7 +7210,7 @@
       <pane xSplit="8" ySplit="3" topLeftCell="J32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J48" sqref="J48"/>
+      <selection pane="bottomRight" activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7263,20 +7263,20 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>564.08000000000004</v>
+        <v>571.13</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.90688102893890676</v>
+        <v>0.91821543408360129</v>
       </c>
       <c r="M3" s="29">
         <f xml:space="preserve"> $J$3 - $L$2</f>
-        <v>-57.919999999999959</v>
+        <v>-50.870000000000005</v>
       </c>
       <c r="N3" s="30">
         <f xml:space="preserve"> $M$3 / $L$2 * 1000</f>
-        <v>-93.118971061093177</v>
+        <v>-81.784565916398719</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -9068,7 +9068,10 @@
         <f xml:space="preserve"> Tableau145[[#This Row],[Samedi]] + 1</f>
         <v>44115</v>
       </c>
-      <c r="J49" s="24"/>
+      <c r="J49" s="24">
+        <f xml:space="preserve"> 7.05</f>
+        <v>7.05</v>
+      </c>
       <c r="K49" s="24"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -9179,7 +9182,7 @@
       <c r="J52" s="24"/>
       <c r="K52" s="24">
         <f>SUM(J48:J52)</f>
-        <v>14.48</v>
+        <v>21.53</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Nous approchons du but !
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -2304,7 +2304,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>44111</v>
+        <v>44120</v>
       </c>
     </row>
   </sheetData>
@@ -7210,7 +7210,7 @@
       <pane xSplit="8" ySplit="3" topLeftCell="J32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J49" sqref="J49"/>
+      <selection pane="bottomRight" activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7263,20 +7263,20 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>571.13</v>
+        <v>587.63</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.91821543408360129</v>
+        <v>0.94474276527331191</v>
       </c>
       <c r="M3" s="29">
         <f xml:space="preserve"> $J$3 - $L$2</f>
-        <v>-50.870000000000005</v>
+        <v>-34.370000000000005</v>
       </c>
       <c r="N3" s="30">
         <f xml:space="preserve"> $M$3 / $L$2 * 1000</f>
-        <v>-81.784565916398719</v>
+        <v>-55.257234726688111</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -9069,8 +9069,8 @@
         <v>44115</v>
       </c>
       <c r="J49" s="24">
-        <f xml:space="preserve"> 7.05</f>
-        <v>7.05</v>
+        <f xml:space="preserve"> 7.05 + 8.98</f>
+        <v>16.03</v>
       </c>
       <c r="K49" s="24"/>
     </row>
@@ -9107,7 +9107,10 @@
         <f xml:space="preserve"> Tableau145[[#This Row],[Samedi]] + 1</f>
         <v>44122</v>
       </c>
-      <c r="J50" s="24"/>
+      <c r="J50" s="24">
+        <f xml:space="preserve"> 7.52</f>
+        <v>7.52</v>
+      </c>
       <c r="K50" s="24"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -9182,7 +9185,7 @@
       <c r="J52" s="24"/>
       <c r="K52" s="24">
         <f>SUM(J48:J52)</f>
-        <v>21.53</v>
+        <v>38.03</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Encore quelques sorties ...
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -2304,7 +2304,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>44120</v>
+        <v>44128</v>
       </c>
     </row>
   </sheetData>
@@ -7210,7 +7210,7 @@
       <pane xSplit="8" ySplit="3" topLeftCell="J32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J50" sqref="J50"/>
+      <selection pane="bottomRight" activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7263,20 +7263,20 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>587.63</v>
+        <v>602.84</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.94474276527331191</v>
+        <v>0.96919614147909972</v>
       </c>
       <c r="M3" s="29">
         <f xml:space="preserve"> $J$3 - $L$2</f>
-        <v>-34.370000000000005</v>
+        <v>-19.159999999999968</v>
       </c>
       <c r="N3" s="30">
         <f xml:space="preserve"> $M$3 / $L$2 * 1000</f>
-        <v>-55.257234726688111</v>
+        <v>-30.80385852090027</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -9108,8 +9108,8 @@
         <v>44122</v>
       </c>
       <c r="J50" s="24">
-        <f xml:space="preserve"> 7.52</f>
-        <v>7.52</v>
+        <f xml:space="preserve"> 7.52 + 8.11</f>
+        <v>15.629999999999999</v>
       </c>
       <c r="K50" s="24"/>
     </row>
@@ -9146,7 +9146,10 @@
         <f xml:space="preserve"> Tableau145[[#This Row],[Samedi]] + 1</f>
         <v>44129</v>
       </c>
-      <c r="J51" s="24"/>
+      <c r="J51" s="24">
+        <f xml:space="preserve"> 7.1</f>
+        <v>7.1</v>
+      </c>
       <c r="K51" s="24"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -9185,7 +9188,7 @@
       <c r="J52" s="24"/>
       <c r="K52" s="24">
         <f>SUM(J48:J52)</f>
-        <v>38.03</v>
+        <v>53.24</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Moins de 20 km ...
...
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -2304,7 +2304,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>44128</v>
+        <v>44130</v>
       </c>
     </row>
   </sheetData>
@@ -7210,7 +7210,7 @@
       <pane xSplit="8" ySplit="3" topLeftCell="J32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J51" sqref="J51"/>
+      <selection pane="bottomRight" activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7263,20 +7263,20 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>602.84</v>
+        <v>610.66000000000008</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.96919614147909972</v>
+        <v>0.98176848874598088</v>
       </c>
       <c r="M3" s="29">
         <f xml:space="preserve"> $J$3 - $L$2</f>
-        <v>-19.159999999999968</v>
+        <v>-11.339999999999918</v>
       </c>
       <c r="N3" s="30">
         <f xml:space="preserve"> $M$3 / $L$2 * 1000</f>
-        <v>-30.80385852090027</v>
+        <v>-18.231511254019161</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -9185,10 +9185,13 @@
         <f xml:space="preserve"> Tableau145[[#This Row],[Samedi]] + 1</f>
         <v>44136</v>
       </c>
-      <c r="J52" s="24"/>
+      <c r="J52" s="24">
+        <f xml:space="preserve"> 7.82</f>
+        <v>7.82</v>
+      </c>
       <c r="K52" s="24">
         <f>SUM(J48:J52)</f>
-        <v>53.24</v>
+        <v>61.06</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
300 km plus loin que la marque
;-)
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles par an.xlsx
+++ b/Src/622 miles/Objectif 622 miles par an.xlsx
@@ -2620,7 +2620,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>44178</v>
+        <v>44193</v>
       </c>
     </row>
   </sheetData>
@@ -7526,7 +7526,7 @@
       <pane xSplit="8" ySplit="3" topLeftCell="J43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J58" sqref="J58"/>
+      <selection pane="bottomRight" activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7579,20 +7579,20 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>770.16</v>
+        <v>812.57999999999993</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>1.2381993569131833</v>
+        <v>1.3063987138263664</v>
       </c>
       <c r="M3" s="29">
         <f xml:space="preserve"> $J$3 - $L$2</f>
-        <v>148.15999999999997</v>
+        <v>190.57999999999993</v>
       </c>
       <c r="N3" s="30">
         <f xml:space="preserve"> $M$3 / $L$2 * 1000</f>
-        <v>238.19935691318324</v>
+        <v>306.39871382636647</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -9779,7 +9779,10 @@
         <f xml:space="preserve"> Tableau145[[#This Row],[Samedi]] + 1</f>
         <v>44185</v>
       </c>
-      <c r="J59" s="24"/>
+      <c r="J59" s="24">
+        <f>6.32 + 13.85</f>
+        <v>20.170000000000002</v>
+      </c>
       <c r="K59" s="24"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -9815,7 +9818,10 @@
         <f xml:space="preserve"> Tableau145[[#This Row],[Samedi]] + 1</f>
         <v>44192</v>
       </c>
-      <c r="J60" s="24"/>
+      <c r="J60" s="24">
+        <f>13.53 + 7.76 + 0.96</f>
+        <v>22.25</v>
+      </c>
       <c r="K60" s="24"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -9854,7 +9860,7 @@
       <c r="J61" s="24"/>
       <c r="K61" s="24">
         <f>SUM(J57:J61)</f>
-        <v>34.07</v>
+        <v>76.490000000000009</v>
       </c>
     </row>
   </sheetData>
@@ -12032,7 +12038,7 @@
         <v>44543</v>
       </c>
       <c r="C59" s="17">
-        <f t="shared" ref="C59:H68" si="17" xml:space="preserve"> 1 + B59</f>
+        <f t="shared" ref="C59:H61" si="17" xml:space="preserve"> 1 + B59</f>
         <v>44544</v>
       </c>
       <c r="D59" s="17">

</xml_diff>